<commit_message>
sync fig 13 with Table 3 Long Running Routine, Sht Running Routine and Zipfian
</commit_message>
<xml_diff>
--- a/resources/excel/genFig15ab (Eurosys2021).xlsx
+++ b/resources/excel/genFig15ab (Eurosys2021).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntellijProjects\SafeHomeFramework\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6AFB07-1EB7-4856-A233-D052FA70BAF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408BBE97-4403-4051-BB05-3130DE9B1D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16903,7 +16903,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16959,8 +16959,8 @@
         <v>0.27014203487258304</v>
       </c>
       <c r="G2" s="5">
-        <f>((B2-E2)/E2)</f>
-        <v>1.8109625471663415</v>
+        <f>((B2)/E2)</f>
+        <v>2.8109625471663415</v>
       </c>
       <c r="H2" s="7">
         <f>((C2-E2)/E2)*100</f>
@@ -16992,8 +16992,8 @@
         <v>0.17822032835708029</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G4" si="0">((B3-E3)/E3)</f>
-        <v>3.0340908583593826</v>
+        <f t="shared" ref="G3:G5" si="0">((B3)/E3)</f>
+        <v>4.0340908583593826</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" ref="H3:H5" si="1">((C3-E3)/E3)*100</f>
@@ -17026,7 +17026,7 @@
       </c>
       <c r="G4" s="5">
         <f t="shared" si="0"/>
-        <v>0.86462207032647687</v>
+        <v>1.8646220703264769</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="1"/>
@@ -17058,8 +17058,8 @@
         <v>5.5144516014022725E-2</v>
       </c>
       <c r="G5" s="5">
-        <f>((B5-E5)/E5)</f>
-        <v>0.4422161954281903</v>
+        <f t="shared" si="0"/>
+        <v>1.4422161954281902</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="1"/>
@@ -17087,14 +17087,14 @@
       </c>
       <c r="B8" s="5">
         <f>G5</f>
-        <v>0.4422161954281903</v>
+        <v>1.4422161954281902</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="5">
         <f>G3</f>
-        <v>3.0340908583593826</v>
+        <v>4.0340908583593826</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>25</v>

</xml_diff>